<commit_message>
Corrected results for CO2
</commit_message>
<xml_diff>
--- a/SetRules.xlsx
+++ b/SetRules.xlsx
@@ -1,28 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
-  <workbookPr backupFile="1" codeName="ThisWorkbook" defaultThemeVersion="166925"/>
+  <workbookPr updateLinks="never" codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Olex\Documents\MANRID\ResLab\Modelling\TIMES\TIMES-IE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1E332CD-8857-4FF5-9ADC-8731981B702F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{69765015-6AAF-4B94-8956-691CCC759B47}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Cover" sheetId="16" r:id="rId1"/>
-    <sheet name="Sets-Comm" sheetId="5" r:id="rId2"/>
-    <sheet name="Sets-Proc" sheetId="11" r:id="rId3"/>
-    <sheet name="IND_Sets-Proc" sheetId="6" r:id="rId4"/>
-    <sheet name="RSD_Sets-Proc" sheetId="9" r:id="rId5"/>
-    <sheet name="TRA_Sets-Proc" sheetId="10" r:id="rId6"/>
-    <sheet name="PWR_Sets-Proc" sheetId="8" r:id="rId7"/>
-    <sheet name="AGR_Sets-Proc" sheetId="14" r:id="rId8"/>
-    <sheet name="SUP_Sets-Proc" sheetId="12" r:id="rId9"/>
-    <sheet name="SRV_Sets-Proc" sheetId="15" r:id="rId10"/>
+    <sheet name="Cover" sheetId="16" r:id="rId3"/>
+    <sheet name="Sets-Comm" sheetId="5" r:id="rId4"/>
+    <sheet name="Sets-Proc" sheetId="11" r:id="rId5"/>
+    <sheet name="IND_Sets-Proc" sheetId="6" r:id="rId6"/>
+    <sheet name="RSD_Sets-Proc" sheetId="9" r:id="rId7"/>
+    <sheet name="TRA_Sets-Proc" sheetId="10" r:id="rId8"/>
+    <sheet name="PWR_Sets-Proc" sheetId="8" r:id="rId9"/>
+    <sheet name="AGR_Sets-Proc" sheetId="14" r:id="rId10"/>
+    <sheet name="SUP_Sets-Proc" sheetId="12" r:id="rId11"/>
+    <sheet name="SRV_Sets-Proc" sheetId="15" r:id="rId12"/>
   </sheets>
   <definedNames>
     <definedName name="__123Graph_AEUMILKPN" hidden="1">#REF!</definedName>
@@ -109,7 +108,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1705" uniqueCount="649">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1705" uniqueCount="651">
   <si>
     <t>~TFM_Psets</t>
   </si>
@@ -636,7 +635,7 @@
     <t>T*CH4*</t>
   </si>
   <si>
-    <t>*CO2*,-*CO2S*</t>
+    <t>*CO2*,-*CO2S*,-TOTCO2*</t>
   </si>
   <si>
     <t>A*CO2*,-*CO2S</t>
@@ -651,7 +650,7 @@
     <t>R*CO2*,-*CO2S</t>
   </si>
   <si>
-    <t>T*CO2*,-*CO2S</t>
+    <t>T*CO2*,-*CO2S,-TOTCO2*</t>
   </si>
   <si>
     <t>*N2O*</t>
@@ -2056,6 +2055,12 @@
   </si>
   <si>
     <t>Olexandr Balyk (UCC, olexandr.balyk@ucc.ie)</t>
+  </si>
+  <si>
+    <t>And</t>
+  </si>
+  <si>
+    <t>Or</t>
   </si>
 </sst>
 </file>
@@ -2065,7 +2070,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="12">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2074,14 +2079,13 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
+      <sz val="10"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
-      <scheme val="minor"/>
     </font>
     <font>
-      <u/>
+      <u val="single"/>
       <sz val="11"/>
       <color theme="10"/>
       <name val="Calibri"/>
@@ -2109,14 +2113,14 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="7" tint="-0.499984740745262"/>
+      <color theme="7" tint="-0.499960005283356"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <u/>
+      <u val="single"/>
       <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -2130,7 +2134,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="7" tint="-0.499984740745262"/>
+      <color theme="7" tint="-0.499960005283356"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -2165,7 +2169,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <fgColor theme="0" tint="-0.149979993700981"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2185,76 +2189,189 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+  <cellStyleXfs count="22">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
+      <alignment/>
+      <protection/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0">
+      <alignment/>
+      <protection/>
+    </xf>
   </cellStyleXfs>
   <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="21" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+      <protection/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="21" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+      <protection/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="21" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+      <protection/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="21" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+      <protection/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="21" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+      <protection/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="21" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+      <protection/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="21" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+      <protection/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="21" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+      <protection/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="21" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+      <protection/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="21" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+      <protection/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="21" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+      <protection/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="2" borderId="0" xfId="21" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="21" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+      <protection/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="21" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+      <protection/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="20" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="21" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
+      <protection/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="21" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="2" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="20" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="3">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="8">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="2" xr:uid="{17C529F0-2ACB-423D-84AA-01D83A782E0E}"/>
+    <cellStyle name="Percent" xfId="15" builtinId="5"/>
+    <cellStyle name="Currency" xfId="16" builtinId="4"/>
+    <cellStyle name="Currency [0]" xfId="17" builtinId="7"/>
+    <cellStyle name="Comma" xfId="18" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="19" builtinId="6"/>
+    <cellStyle name="Hyperlink" xfId="20" builtinId="8"/>
+    <cellStyle name="Normal 2" xfId="21"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -2267,7 +2384,7 @@
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
@@ -2286,7 +2403,7 @@
         <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F4793B0C-7E95-455C-B0CB-1A9B2502D62C}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{f4793b0c-7e95-455c-b0cb-1a9b2502d62c}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2295,19 +2412,17 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:blip r:embed="rId1"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9525" y="1"/>
-          <a:ext cx="5796000" cy="2324211"/>
+          <a:off x="9525" y="0"/>
+          <a:ext cx="5800725" cy="2324100"/>
         </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
+        <a:prstGeom prst="rect"/>
       </xdr:spPr>
     </xdr:pic>
     <xdr:clientData/>
@@ -2330,7 +2445,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{784447AE-1FD0-4F28-A1A5-EE6260431F6B}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{784447ae-1fd0-4f28-a1a5-ee6260431f6b}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2338,25 +2453,19 @@
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
-      <xdr:blipFill rotWithShape="1">
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:srcRect l="4620" t="8935" r="7748" b="12927"/>
-        <a:stretch/>
+      <xdr:blipFill>
+        <a:blip r:embed="rId2"/>
+        <a:srcRect l="4617" t="8932" r="7745" b="12924"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
           <a:off x="19050" y="8810625"/>
-          <a:ext cx="1431433" cy="576000"/>
+          <a:ext cx="1428750" cy="571500"/>
         </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
+        <a:prstGeom prst="rect"/>
       </xdr:spPr>
     </xdr:pic>
     <xdr:clientData/>
@@ -2379,7 +2488,7 @@
         <xdr:cNvPr id="4" name="Picture 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{491EA09E-8916-42B6-AFF9-6AE648928F62}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{491ea09e-8916-42b6-aff9-6ae648928f62}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2388,25 +2497,17 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3" cstate="print">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
+        <a:blip r:embed="rId3"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1957123" y="8810625"/>
-          <a:ext cx="1250988" cy="576000"/>
+          <a:off x="1952625" y="8810625"/>
+          <a:ext cx="1247775" cy="571500"/>
         </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
+        <a:prstGeom prst="rect"/>
       </xdr:spPr>
     </xdr:pic>
     <xdr:clientData/>
@@ -2429,7 +2530,7 @@
         <xdr:cNvPr id="5" name="Picture 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{049B1B57-E70B-46F9-901A-CE09A3B75F2C}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{049b1b57-e70b-46f9-901a-ce09a3b75f2c}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2438,25 +2539,17 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4" cstate="print">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
+        <a:blip r:embed="rId4"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3733801" y="8810625"/>
-          <a:ext cx="2018073" cy="576000"/>
+          <a:off x="3733800" y="8810625"/>
+          <a:ext cx="2019300" cy="571500"/>
         </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
+        <a:prstGeom prst="rect"/>
       </xdr:spPr>
     </xdr:pic>
     <xdr:clientData/>
@@ -2479,7 +2572,7 @@
         <xdr:cNvPr id="6" name="Picture 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2A8091D1-74BF-4EFB-AAD8-850904C730D0}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2a8091d1-74bf-4efb-aad8-850904c730d0}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2487,25 +2580,19 @@
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
-      <xdr:blipFill rotWithShape="1">
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5" cstate="print">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:srcRect l="1369" t="6565" r="4012" b="6338"/>
-        <a:stretch/>
+      <xdr:blipFill>
+        <a:blip r:embed="rId5"/>
+        <a:srcRect l="1367" t="6562" r="4010" b="6335"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3628275" y="7962900"/>
-          <a:ext cx="1400925" cy="576000"/>
+          <a:off x="3629025" y="7962900"/>
+          <a:ext cx="1400175" cy="571500"/>
         </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
+        <a:prstGeom prst="rect"/>
       </xdr:spPr>
     </xdr:pic>
     <xdr:clientData/>
@@ -2528,36 +2615,27 @@
         <xdr:cNvPr id="7" name="Picture 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8AB27DD0-3AE8-4401-AAF8-48085C11883C}"/>
-            </a:ext>
-            <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
-              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{B1489C0F-1609-4587-A5BA-D0B99739EA08}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8ab27dd0-3ae8-4401-aaf8-48085c11883c}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
         <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+          <a:picLocks noChangeArrowheads="1" noChangeAspect="1"/>
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
-      <xdr:blipFill rotWithShape="1">
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6" cstate="print">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:srcRect l="4000" t="26200" r="4000" b="26199"/>
-        <a:stretch/>
+      <xdr:blipFill>
+        <a:blip r:embed="rId6"/>
+        <a:srcRect l="3997" t="26197" r="3997" b="26196"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
           <a:off x="666750" y="8077200"/>
           <a:ext cx="1676400" cy="428625"/>
         </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
+        <a:prstGeom prst="rect"/>
         <a:noFill/>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
@@ -2871,28 +2949,28 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A254A0F-7158-4F85-B7C3-36851FAE9E89}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A254A0F-7158-4F85-B7C3-36851FAE9E89}">
   <sheetPr codeName="Sheet10"/>
   <dimension ref="A1:Z99"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0" topLeftCell="A1">
+      <selection pane="topLeft" activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.85428571428571" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="4" width="21.7109375" customWidth="1"/>
-    <col min="5" max="6" width="14.140625" customWidth="1"/>
-    <col min="7" max="7" width="12.140625" customWidth="1"/>
-    <col min="8" max="10" width="8.140625" customWidth="1"/>
-    <col min="11" max="11" width="9.7109375" customWidth="1"/>
-    <col min="12" max="12" width="8.140625" customWidth="1"/>
+    <col min="1" max="4" width="21.7142857142857" customWidth="1"/>
+    <col min="5" max="6" width="14.1428571428571" customWidth="1"/>
+    <col min="7" max="7" width="12.1428571428571" customWidth="1"/>
+    <col min="8" max="10" width="8.14285714285714" customWidth="1"/>
+    <col min="11" max="11" width="9.71428571428571" customWidth="1"/>
+    <col min="12" max="12" width="8.14285714285714" customWidth="1"/>
     <col min="13" max="13" width="10" customWidth="1"/>
-    <col min="14" max="14" width="11.42578125" customWidth="1"/>
-    <col min="15" max="15" width="13.42578125" customWidth="1"/>
+    <col min="14" max="14" width="11.4285714285714" customWidth="1"/>
+    <col min="15" max="15" width="13.4285714285714" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:26" ht="15">
       <c r="A1" s="2"/>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -2920,7 +2998,7 @@
       <c r="Y1" s="3"/>
       <c r="Z1" s="3"/>
     </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:26" ht="15">
       <c r="A2" s="2"/>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
@@ -2948,7 +3026,7 @@
       <c r="Y2" s="3"/>
       <c r="Z2" s="3"/>
     </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:26" ht="15">
       <c r="A3" s="2"/>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
@@ -2976,7 +3054,7 @@
       <c r="Y3" s="3"/>
       <c r="Z3" s="3"/>
     </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:26" ht="15">
       <c r="A4" s="2"/>
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
@@ -3004,7 +3082,7 @@
       <c r="Y4" s="3"/>
       <c r="Z4" s="3"/>
     </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:26" ht="15">
       <c r="A5" s="2"/>
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
@@ -3032,7 +3110,7 @@
       <c r="Y5" s="3"/>
       <c r="Z5" s="3"/>
     </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:26" ht="15">
       <c r="A6" s="2"/>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
@@ -3060,7 +3138,7 @@
       <c r="Y6" s="3"/>
       <c r="Z6" s="3"/>
     </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:26" ht="15">
       <c r="A7" s="2"/>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
@@ -3088,7 +3166,7 @@
       <c r="Y7" s="3"/>
       <c r="Z7" s="3"/>
     </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:26" ht="15">
       <c r="A8" s="2"/>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
@@ -3116,7 +3194,7 @@
       <c r="Y8" s="3"/>
       <c r="Z8" s="3"/>
     </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:26" ht="15">
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
@@ -3144,7 +3222,7 @@
       <c r="Y9" s="3"/>
       <c r="Z9" s="3"/>
     </row>
-    <row r="10" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:26" ht="15">
       <c r="A10" s="2"/>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
@@ -3172,7 +3250,7 @@
       <c r="Y10" s="3"/>
       <c r="Z10" s="3"/>
     </row>
-    <row r="11" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:26" ht="15">
       <c r="A11" s="2"/>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
@@ -3200,7 +3278,7 @@
       <c r="Y11" s="3"/>
       <c r="Z11" s="3"/>
     </row>
-    <row r="12" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:26" ht="15">
       <c r="A12" s="2"/>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
@@ -3228,7 +3306,7 @@
       <c r="Y12" s="3"/>
       <c r="Z12" s="3"/>
     </row>
-    <row r="13" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:26" ht="15">
       <c r="A13" s="2"/>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
@@ -3256,7 +3334,7 @@
       <c r="Y13" s="3"/>
       <c r="Z13" s="3"/>
     </row>
-    <row r="14" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:26" ht="15">
       <c r="A14" s="2"/>
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
@@ -3284,7 +3362,7 @@
       <c r="Y14" s="3"/>
       <c r="Z14" s="3"/>
     </row>
-    <row r="15" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:26" ht="15">
       <c r="A15" s="2"/>
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
@@ -3312,7 +3390,7 @@
       <c r="Y15" s="3"/>
       <c r="Z15" s="3"/>
     </row>
-    <row r="16" spans="1:26" ht="102.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:26" ht="102.75" customHeight="1">
       <c r="A16" s="18" t="s">
         <v>633</v>
       </c>
@@ -3342,7 +3420,7 @@
       <c r="Y16" s="3"/>
       <c r="Z16" s="3"/>
     </row>
-    <row r="17" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:26" ht="17.25" customHeight="1">
       <c r="A17" s="6"/>
       <c r="B17" s="6"/>
       <c r="C17" s="6"/>
@@ -3370,7 +3448,7 @@
       <c r="Y17" s="3"/>
       <c r="Z17" s="3"/>
     </row>
-    <row r="18" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:26" ht="17.25" customHeight="1">
       <c r="A18" s="6"/>
       <c r="B18" s="6"/>
       <c r="C18" s="6"/>
@@ -3398,7 +3476,7 @@
       <c r="Y18" s="3"/>
       <c r="Z18" s="3"/>
     </row>
-    <row r="19" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:26" ht="17.25" customHeight="1">
       <c r="A19" s="9" t="s">
         <v>634</v>
       </c>
@@ -3430,7 +3508,7 @@
       <c r="Y19" s="3"/>
       <c r="Z19" s="3"/>
     </row>
-    <row r="20" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:26" ht="17.25" customHeight="1">
       <c r="A20" s="9" t="s">
         <v>635</v>
       </c>
@@ -3462,7 +3540,7 @@
       <c r="Y20" s="3"/>
       <c r="Z20" s="3"/>
     </row>
-    <row r="21" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:26" ht="17.25" customHeight="1">
       <c r="A21" s="9" t="s">
         <v>636</v>
       </c>
@@ -3494,7 +3572,7 @@
       <c r="Y21" s="3"/>
       <c r="Z21" s="3"/>
     </row>
-    <row r="22" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:26" ht="17.25" customHeight="1">
       <c r="A22" s="9"/>
       <c r="B22" s="12"/>
       <c r="C22" s="12"/>
@@ -3522,7 +3600,7 @@
       <c r="Y22" s="3"/>
       <c r="Z22" s="3"/>
     </row>
-    <row r="23" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:26" ht="17.25" customHeight="1">
       <c r="A23" s="9" t="s">
         <v>637</v>
       </c>
@@ -3554,7 +3632,7 @@
       <c r="Y23" s="3"/>
       <c r="Z23" s="3"/>
     </row>
-    <row r="24" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:26" ht="17.25" customHeight="1">
       <c r="A24" s="9"/>
       <c r="B24" s="12"/>
       <c r="C24" s="12"/>
@@ -3582,7 +3660,7 @@
       <c r="Y24" s="3"/>
       <c r="Z24" s="3"/>
     </row>
-    <row r="25" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:26" ht="17.25" customHeight="1">
       <c r="A25" s="9"/>
       <c r="B25" s="12"/>
       <c r="C25" s="12"/>
@@ -3610,7 +3688,7 @@
       <c r="Y25" s="3"/>
       <c r="Z25" s="3"/>
     </row>
-    <row r="26" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:26" ht="17.25" customHeight="1">
       <c r="A26" s="9" t="s">
         <v>638</v>
       </c>
@@ -3642,7 +3720,7 @@
       <c r="Y26" s="3"/>
       <c r="Z26" s="3"/>
     </row>
-    <row r="27" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:26" ht="17.25" customHeight="1">
       <c r="A27" s="9"/>
       <c r="B27" s="12"/>
       <c r="C27" s="12"/>
@@ -3670,7 +3748,7 @@
       <c r="Y27" s="3"/>
       <c r="Z27" s="3"/>
     </row>
-    <row r="28" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:26" ht="17.25" customHeight="1">
       <c r="A28" s="9"/>
       <c r="B28" s="12"/>
       <c r="C28" s="12"/>
@@ -3698,7 +3776,7 @@
       <c r="Y28" s="3"/>
       <c r="Z28" s="3"/>
     </row>
-    <row r="29" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:26" ht="17.25" customHeight="1">
       <c r="A29" s="9" t="s">
         <v>639</v>
       </c>
@@ -3730,7 +3808,7 @@
       <c r="Y29" s="3"/>
       <c r="Z29" s="3"/>
     </row>
-    <row r="30" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:26" ht="17.25" customHeight="1">
       <c r="A30" s="9" t="s">
         <v>640</v>
       </c>
@@ -3762,7 +3840,7 @@
       <c r="Y30" s="3"/>
       <c r="Z30" s="3"/>
     </row>
-    <row r="31" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:26" ht="17.25" customHeight="1">
       <c r="A31" s="9" t="s">
         <v>642</v>
       </c>
@@ -3794,7 +3872,7 @@
       <c r="Y31" s="3"/>
       <c r="Z31" s="3"/>
     </row>
-    <row r="32" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:26" ht="17.25" customHeight="1">
       <c r="A32" s="15"/>
       <c r="B32" s="16" t="s">
         <v>644</v>
@@ -3824,7 +3902,7 @@
       <c r="Y32" s="3"/>
       <c r="Z32" s="3"/>
     </row>
-    <row r="33" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:26" ht="15">
       <c r="A33" s="2"/>
       <c r="B33" s="2"/>
       <c r="C33" s="2"/>
@@ -3852,7 +3930,7 @@
       <c r="Y33" s="3"/>
       <c r="Z33" s="3"/>
     </row>
-    <row r="34" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:26" ht="15">
       <c r="A34" s="2"/>
       <c r="B34" s="2"/>
       <c r="C34" s="2"/>
@@ -3880,7 +3958,7 @@
       <c r="Y34" s="3"/>
       <c r="Z34" s="3"/>
     </row>
-    <row r="35" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:26" ht="15">
       <c r="A35" s="2"/>
       <c r="B35" s="2"/>
       <c r="C35" s="2"/>
@@ -3908,7 +3986,7 @@
       <c r="Y35" s="3"/>
       <c r="Z35" s="3"/>
     </row>
-    <row r="36" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:26" ht="15">
       <c r="A36" s="2"/>
       <c r="B36" s="2"/>
       <c r="C36" s="2"/>
@@ -3936,7 +4014,7 @@
       <c r="Y36" s="3"/>
       <c r="Z36" s="3"/>
     </row>
-    <row r="37" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:26" ht="15">
       <c r="A37" s="2"/>
       <c r="B37" s="2"/>
       <c r="C37" s="2"/>
@@ -3964,7 +4042,7 @@
       <c r="Y37" s="3"/>
       <c r="Z37" s="3"/>
     </row>
-    <row r="38" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:26" ht="15">
       <c r="A38" s="2"/>
       <c r="B38" s="2"/>
       <c r="C38" s="2"/>
@@ -3992,7 +4070,7 @@
       <c r="Y38" s="3"/>
       <c r="Z38" s="3"/>
     </row>
-    <row r="39" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:26" ht="15">
       <c r="A39" s="2"/>
       <c r="B39" s="2"/>
       <c r="C39" s="2"/>
@@ -4020,7 +4098,7 @@
       <c r="Y39" s="3"/>
       <c r="Z39" s="3"/>
     </row>
-    <row r="40" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:26" ht="15">
       <c r="A40" s="2"/>
       <c r="B40" s="2"/>
       <c r="C40" s="2"/>
@@ -4048,7 +4126,7 @@
       <c r="Y40" s="3"/>
       <c r="Z40" s="3"/>
     </row>
-    <row r="41" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:26" ht="15">
       <c r="A41" s="2"/>
       <c r="B41" s="2"/>
       <c r="C41" s="2"/>
@@ -4076,7 +4154,7 @@
       <c r="Y41" s="3"/>
       <c r="Z41" s="3"/>
     </row>
-    <row r="42" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:26" ht="15">
       <c r="A42" s="2"/>
       <c r="B42" s="2"/>
       <c r="C42" s="2"/>
@@ -4104,7 +4182,7 @@
       <c r="Y42" s="3"/>
       <c r="Z42" s="3"/>
     </row>
-    <row r="43" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:26" ht="15">
       <c r="A43" s="3"/>
       <c r="B43" s="3"/>
       <c r="C43" s="3"/>
@@ -4132,7 +4210,7 @@
       <c r="Y43" s="3"/>
       <c r="Z43" s="3"/>
     </row>
-    <row r="44" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:26" ht="15">
       <c r="A44" s="3"/>
       <c r="B44" s="3"/>
       <c r="C44" s="3"/>
@@ -4160,7 +4238,7 @@
       <c r="Y44" s="3"/>
       <c r="Z44" s="3"/>
     </row>
-    <row r="45" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:26" ht="15">
       <c r="A45" s="3"/>
       <c r="B45" s="3"/>
       <c r="C45" s="3"/>
@@ -4188,7 +4266,7 @@
       <c r="Y45" s="3"/>
       <c r="Z45" s="3"/>
     </row>
-    <row r="46" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:26" ht="15">
       <c r="A46" s="3"/>
       <c r="B46" s="3"/>
       <c r="C46" s="3"/>
@@ -4216,7 +4294,7 @@
       <c r="Y46" s="3"/>
       <c r="Z46" s="3"/>
     </row>
-    <row r="47" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:26" ht="15">
       <c r="A47" s="3"/>
       <c r="B47" s="3"/>
       <c r="C47" s="3"/>
@@ -4244,7 +4322,7 @@
       <c r="Y47" s="3"/>
       <c r="Z47" s="3"/>
     </row>
-    <row r="48" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:26" ht="15">
       <c r="A48" s="3"/>
       <c r="B48" s="3"/>
       <c r="C48" s="3"/>
@@ -4272,7 +4350,7 @@
       <c r="Y48" s="3"/>
       <c r="Z48" s="3"/>
     </row>
-    <row r="49" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:26" ht="15">
       <c r="A49" s="3"/>
       <c r="B49" s="3"/>
       <c r="C49" s="3"/>
@@ -4300,7 +4378,7 @@
       <c r="Y49" s="3"/>
       <c r="Z49" s="3"/>
     </row>
-    <row r="50" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:26" ht="15">
       <c r="A50" s="3"/>
       <c r="B50" s="3"/>
       <c r="C50" s="3"/>
@@ -4328,7 +4406,7 @@
       <c r="Y50" s="3"/>
       <c r="Z50" s="3"/>
     </row>
-    <row r="51" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:26" ht="15">
       <c r="A51" s="3"/>
       <c r="B51" s="3"/>
       <c r="C51" s="3"/>
@@ -4356,7 +4434,7 @@
       <c r="Y51" s="3"/>
       <c r="Z51" s="3"/>
     </row>
-    <row r="52" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:26" ht="15">
       <c r="A52" s="3"/>
       <c r="B52" s="3"/>
       <c r="C52" s="3"/>
@@ -4384,7 +4462,7 @@
       <c r="Y52" s="3"/>
       <c r="Z52" s="3"/>
     </row>
-    <row r="53" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:26" ht="15">
       <c r="A53" s="3"/>
       <c r="B53" s="3"/>
       <c r="C53" s="3"/>
@@ -4412,7 +4490,7 @@
       <c r="Y53" s="3"/>
       <c r="Z53" s="3"/>
     </row>
-    <row r="54" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:26" ht="15">
       <c r="A54" s="3"/>
       <c r="B54" s="3"/>
       <c r="C54" s="3"/>
@@ -4440,7 +4518,7 @@
       <c r="Y54" s="3"/>
       <c r="Z54" s="3"/>
     </row>
-    <row r="55" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:26" ht="15">
       <c r="A55" s="3"/>
       <c r="B55" s="3"/>
       <c r="C55" s="3"/>
@@ -4468,7 +4546,7 @@
       <c r="Y55" s="3"/>
       <c r="Z55" s="3"/>
     </row>
-    <row r="56" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:26" ht="15">
       <c r="A56" s="3"/>
       <c r="B56" s="3"/>
       <c r="C56" s="3"/>
@@ -4496,7 +4574,7 @@
       <c r="Y56" s="3"/>
       <c r="Z56" s="3"/>
     </row>
-    <row r="57" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:26" ht="15">
       <c r="A57" s="3"/>
       <c r="B57" s="3"/>
       <c r="C57" s="3"/>
@@ -4524,7 +4602,7 @@
       <c r="Y57" s="3"/>
       <c r="Z57" s="3"/>
     </row>
-    <row r="58" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:26" ht="15">
       <c r="A58" s="3"/>
       <c r="B58" s="3"/>
       <c r="C58" s="3"/>
@@ -4552,7 +4630,7 @@
       <c r="Y58" s="3"/>
       <c r="Z58" s="3"/>
     </row>
-    <row r="59" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:26" ht="15">
       <c r="A59" s="3"/>
       <c r="B59" s="3"/>
       <c r="C59" s="3"/>
@@ -4580,7 +4658,7 @@
       <c r="Y59" s="3"/>
       <c r="Z59" s="3"/>
     </row>
-    <row r="60" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:26" ht="15">
       <c r="A60" s="3"/>
       <c r="B60" s="3"/>
       <c r="C60" s="3"/>
@@ -4608,7 +4686,7 @@
       <c r="Y60" s="3"/>
       <c r="Z60" s="3"/>
     </row>
-    <row r="61" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:26" ht="15">
       <c r="A61" s="3"/>
       <c r="B61" s="3"/>
       <c r="C61" s="3"/>
@@ -4636,7 +4714,7 @@
       <c r="Y61" s="3"/>
       <c r="Z61" s="3"/>
     </row>
-    <row r="62" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:26" ht="15">
       <c r="A62" s="3"/>
       <c r="B62" s="3"/>
       <c r="C62" s="3"/>
@@ -4664,7 +4742,7 @@
       <c r="Y62" s="3"/>
       <c r="Z62" s="3"/>
     </row>
-    <row r="63" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:26" ht="15">
       <c r="A63" s="3"/>
       <c r="B63" s="3"/>
       <c r="C63" s="3"/>
@@ -4692,7 +4770,7 @@
       <c r="Y63" s="3"/>
       <c r="Z63" s="3"/>
     </row>
-    <row r="64" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:26" ht="15">
       <c r="A64" s="3"/>
       <c r="B64" s="3"/>
       <c r="C64" s="3"/>
@@ -4720,7 +4798,7 @@
       <c r="Y64" s="3"/>
       <c r="Z64" s="3"/>
     </row>
-    <row r="65" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:26" ht="15">
       <c r="A65" s="3"/>
       <c r="B65" s="3"/>
       <c r="C65" s="3"/>
@@ -4748,7 +4826,7 @@
       <c r="Y65" s="3"/>
       <c r="Z65" s="3"/>
     </row>
-    <row r="66" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:26" ht="15">
       <c r="A66" s="3"/>
       <c r="B66" s="3"/>
       <c r="C66" s="3"/>
@@ -4776,7 +4854,7 @@
       <c r="Y66" s="3"/>
       <c r="Z66" s="3"/>
     </row>
-    <row r="67" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:26" ht="15">
       <c r="A67" s="3"/>
       <c r="B67" s="3"/>
       <c r="C67" s="3"/>
@@ -4804,7 +4882,7 @@
       <c r="Y67" s="3"/>
       <c r="Z67" s="3"/>
     </row>
-    <row r="68" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:26" ht="15">
       <c r="A68" s="3"/>
       <c r="B68" s="3"/>
       <c r="C68" s="3"/>
@@ -4832,7 +4910,7 @@
       <c r="Y68" s="3"/>
       <c r="Z68" s="3"/>
     </row>
-    <row r="69" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:26" ht="15">
       <c r="A69" s="3"/>
       <c r="B69" s="3"/>
       <c r="C69" s="3"/>
@@ -4860,7 +4938,7 @@
       <c r="Y69" s="3"/>
       <c r="Z69" s="3"/>
     </row>
-    <row r="70" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:26" ht="15">
       <c r="A70" s="3"/>
       <c r="B70" s="3"/>
       <c r="C70" s="3"/>
@@ -4888,7 +4966,7 @@
       <c r="Y70" s="3"/>
       <c r="Z70" s="3"/>
     </row>
-    <row r="71" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:26" ht="15">
       <c r="A71" s="3"/>
       <c r="B71" s="3"/>
       <c r="C71" s="3"/>
@@ -4916,7 +4994,7 @@
       <c r="Y71" s="3"/>
       <c r="Z71" s="3"/>
     </row>
-    <row r="72" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:26" ht="15">
       <c r="A72" s="3"/>
       <c r="B72" s="3"/>
       <c r="C72" s="3"/>
@@ -4944,7 +5022,7 @@
       <c r="Y72" s="3"/>
       <c r="Z72" s="3"/>
     </row>
-    <row r="73" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:26" ht="15">
       <c r="A73" s="3"/>
       <c r="B73" s="3"/>
       <c r="C73" s="3"/>
@@ -4972,7 +5050,7 @@
       <c r="Y73" s="3"/>
       <c r="Z73" s="3"/>
     </row>
-    <row r="74" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:26" ht="15">
       <c r="A74" s="3"/>
       <c r="B74" s="3"/>
       <c r="C74" s="3"/>
@@ -5000,7 +5078,7 @@
       <c r="Y74" s="3"/>
       <c r="Z74" s="3"/>
     </row>
-    <row r="75" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:26" ht="15">
       <c r="A75" s="3"/>
       <c r="B75" s="3"/>
       <c r="C75" s="3"/>
@@ -5028,7 +5106,7 @@
       <c r="Y75" s="3"/>
       <c r="Z75" s="3"/>
     </row>
-    <row r="76" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:26" ht="15">
       <c r="A76" s="3"/>
       <c r="B76" s="3"/>
       <c r="C76" s="3"/>
@@ -5056,7 +5134,7 @@
       <c r="Y76" s="3"/>
       <c r="Z76" s="3"/>
     </row>
-    <row r="77" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:26" ht="15">
       <c r="A77" s="3"/>
       <c r="B77" s="3"/>
       <c r="C77" s="3"/>
@@ -5084,7 +5162,7 @@
       <c r="Y77" s="3"/>
       <c r="Z77" s="3"/>
     </row>
-    <row r="78" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:26" ht="15">
       <c r="A78" s="3"/>
       <c r="B78" s="3"/>
       <c r="C78" s="3"/>
@@ -5112,7 +5190,7 @@
       <c r="Y78" s="3"/>
       <c r="Z78" s="3"/>
     </row>
-    <row r="79" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:26" ht="15">
       <c r="A79" s="3"/>
       <c r="B79" s="3"/>
       <c r="C79" s="3"/>
@@ -5140,7 +5218,7 @@
       <c r="Y79" s="3"/>
       <c r="Z79" s="3"/>
     </row>
-    <row r="80" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:26" ht="15">
       <c r="A80" s="3"/>
       <c r="B80" s="3"/>
       <c r="C80" s="3"/>
@@ -5168,7 +5246,7 @@
       <c r="Y80" s="3"/>
       <c r="Z80" s="3"/>
     </row>
-    <row r="81" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:26" ht="15">
       <c r="A81" s="3"/>
       <c r="B81" s="3"/>
       <c r="C81" s="3"/>
@@ -5196,7 +5274,7 @@
       <c r="Y81" s="3"/>
       <c r="Z81" s="3"/>
     </row>
-    <row r="82" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:26" ht="15">
       <c r="A82" s="3"/>
       <c r="B82" s="3"/>
       <c r="C82" s="3"/>
@@ -5224,7 +5302,7 @@
       <c r="Y82" s="3"/>
       <c r="Z82" s="3"/>
     </row>
-    <row r="83" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:26" ht="15">
       <c r="A83" s="3"/>
       <c r="B83" s="3"/>
       <c r="C83" s="3"/>
@@ -5252,7 +5330,7 @@
       <c r="Y83" s="3"/>
       <c r="Z83" s="3"/>
     </row>
-    <row r="84" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:26" ht="15">
       <c r="A84" s="3"/>
       <c r="B84" s="3"/>
       <c r="C84" s="3"/>
@@ -5280,7 +5358,7 @@
       <c r="Y84" s="3"/>
       <c r="Z84" s="3"/>
     </row>
-    <row r="85" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:26" ht="15">
       <c r="A85" s="3"/>
       <c r="B85" s="3"/>
       <c r="C85" s="3"/>
@@ -5308,7 +5386,7 @@
       <c r="Y85" s="3"/>
       <c r="Z85" s="3"/>
     </row>
-    <row r="86" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:26" ht="15">
       <c r="A86" s="3"/>
       <c r="B86" s="3"/>
       <c r="C86" s="3"/>
@@ -5336,7 +5414,7 @@
       <c r="Y86" s="3"/>
       <c r="Z86" s="3"/>
     </row>
-    <row r="87" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:26" ht="15">
       <c r="A87" s="3"/>
       <c r="B87" s="3"/>
       <c r="C87" s="3"/>
@@ -5364,7 +5442,7 @@
       <c r="Y87" s="3"/>
       <c r="Z87" s="3"/>
     </row>
-    <row r="88" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:26" ht="15">
       <c r="A88" s="3"/>
       <c r="B88" s="3"/>
       <c r="C88" s="3"/>
@@ -5392,7 +5470,7 @@
       <c r="Y88" s="3"/>
       <c r="Z88" s="3"/>
     </row>
-    <row r="89" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:26" ht="15">
       <c r="A89" s="3"/>
       <c r="B89" s="3"/>
       <c r="C89" s="3"/>
@@ -5420,7 +5498,7 @@
       <c r="Y89" s="3"/>
       <c r="Z89" s="3"/>
     </row>
-    <row r="90" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:26" ht="15">
       <c r="A90" s="3"/>
       <c r="B90" s="3"/>
       <c r="C90" s="3"/>
@@ -5448,7 +5526,7 @@
       <c r="Y90" s="3"/>
       <c r="Z90" s="3"/>
     </row>
-    <row r="91" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:26" ht="15">
       <c r="A91" s="3"/>
       <c r="B91" s="3"/>
       <c r="C91" s="3"/>
@@ -5476,7 +5554,7 @@
       <c r="Y91" s="3"/>
       <c r="Z91" s="3"/>
     </row>
-    <row r="92" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:26" ht="15">
       <c r="A92" s="3"/>
       <c r="B92" s="3"/>
       <c r="C92" s="3"/>
@@ -5504,7 +5582,7 @@
       <c r="Y92" s="3"/>
       <c r="Z92" s="3"/>
     </row>
-    <row r="93" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:26" ht="15">
       <c r="A93" s="3"/>
       <c r="B93" s="3"/>
       <c r="C93" s="3"/>
@@ -5532,7 +5610,7 @@
       <c r="Y93" s="3"/>
       <c r="Z93" s="3"/>
     </row>
-    <row r="94" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:26" ht="15">
       <c r="A94" s="3"/>
       <c r="B94" s="3"/>
       <c r="C94" s="3"/>
@@ -5560,7 +5638,7 @@
       <c r="Y94" s="3"/>
       <c r="Z94" s="3"/>
     </row>
-    <row r="95" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:26" ht="15">
       <c r="A95" s="3"/>
       <c r="B95" s="3"/>
       <c r="C95" s="3"/>
@@ -5588,7 +5666,7 @@
       <c r="Y95" s="3"/>
       <c r="Z95" s="3"/>
     </row>
-    <row r="96" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:26" ht="15">
       <c r="A96" s="3"/>
       <c r="B96" s="3"/>
       <c r="C96" s="3"/>
@@ -5616,7 +5694,7 @@
       <c r="Y96" s="3"/>
       <c r="Z96" s="3"/>
     </row>
-    <row r="97" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:26" ht="15">
       <c r="A97" s="3"/>
       <c r="B97" s="3"/>
       <c r="C97" s="3"/>
@@ -5644,7 +5722,7 @@
       <c r="Y97" s="3"/>
       <c r="Z97" s="3"/>
     </row>
-    <row r="98" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:26" ht="15">
       <c r="A98" s="3"/>
       <c r="B98" s="3"/>
       <c r="C98" s="3"/>
@@ -5672,7 +5750,7 @@
       <c r="Y98" s="3"/>
       <c r="Z98" s="3"/>
     </row>
-    <row r="99" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:26" ht="15">
       <c r="A99" s="3"/>
       <c r="B99" s="3"/>
       <c r="C99" s="3"/>
@@ -5711,40 +5789,40 @@
     <mergeCell ref="B30:D30"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="B30" r:id="rId1" xr:uid="{7C4949C3-8590-458B-B2D3-98B4CE2A4156}"/>
-    <hyperlink ref="B32" r:id="rId2" xr:uid="{11085E39-260B-4B51-8A4C-480062017CCE}"/>
+    <hyperlink ref="B30" r:id="rId1" display="https://github.com/MaREI-EPMG/TIMES-Ireland-model"/>
+    <hyperlink ref="B32" r:id="rId2" display="https://creativecommons.org/licenses/by-nc-sa/4.0/"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
-  <drawing r:id="rId4"/>
+  <pageSetup orientation="portrait" paperSize="9" r:id="rId4"/>
+  <drawing r:id="rId3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55F4EBB5-8F5D-4492-A870-22D6545A1D24}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55F4EBB5-8F5D-4492-A870-22D6545A1D24}">
   <sheetPr codeName="Sheet9">
     <tabColor rgb="FF92D050"/>
   </sheetPr>
   <dimension ref="A1:L19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H31" sqref="H31"/>
+    <sheetView workbookViewId="0" topLeftCell="A1">
+      <selection pane="topLeft" activeCell="H31" sqref="H31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="4" max="4" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="29.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="57.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.2857142857143" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="29.1428571428571" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.8571428571429" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="57.8571428571429" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" ht="15">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" ht="15">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -5782,7 +5860,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" ht="15">
       <c r="A3" s="1"/>
       <c r="B3" t="s">
         <v>546</v>
@@ -5809,7 +5887,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:11" ht="15">
       <c r="B4" t="s">
         <v>546</v>
       </c>
@@ -5835,7 +5913,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:11" ht="15">
       <c r="B5" t="s">
         <v>546</v>
       </c>
@@ -5861,7 +5939,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:11" ht="15">
       <c r="B6" t="s">
         <v>546</v>
       </c>
@@ -5887,7 +5965,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:11" ht="15">
       <c r="B7" t="s">
         <v>546</v>
       </c>
@@ -5913,7 +5991,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:11" ht="15">
       <c r="B8" t="s">
         <v>546</v>
       </c>
@@ -5939,7 +6017,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:11" ht="15">
       <c r="B9" t="s">
         <v>546</v>
       </c>
@@ -5965,7 +6043,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:11" ht="15">
       <c r="B10" t="s">
         <v>546</v>
       </c>
@@ -5991,7 +6069,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:11" ht="15">
       <c r="B11" t="s">
         <v>546</v>
       </c>
@@ -6017,7 +6095,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:11" ht="15">
       <c r="B12" t="s">
         <v>546</v>
       </c>
@@ -6043,7 +6121,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" ht="15">
       <c r="A13" t="s">
         <v>45</v>
       </c>
@@ -6072,7 +6150,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" ht="15">
       <c r="A14" t="s">
         <v>45</v>
       </c>
@@ -6101,7 +6179,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" ht="15">
       <c r="A15" t="s">
         <v>45</v>
       </c>
@@ -6130,7 +6208,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" ht="15">
       <c r="A16" t="s">
         <v>45</v>
       </c>
@@ -6159,7 +6237,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="17" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:11" ht="15">
       <c r="B17" t="s">
         <v>546</v>
       </c>
@@ -6185,7 +6263,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:11" ht="15">
       <c r="B18" t="s">
         <v>606</v>
       </c>
@@ -6211,7 +6289,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="19" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:11" ht="15">
       <c r="B19" t="s">
         <v>608</v>
       </c>
@@ -6243,28 +6321,28 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92FCDF15-1442-474A-ACC7-D199AB8A1E18}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92FCDF15-1442-474A-ACC7-D199AB8A1E18}">
   <sheetPr codeName="Sheet1">
     <tabColor rgb="FF92D050"/>
   </sheetPr>
   <dimension ref="A1:J79"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="L25" sqref="L25"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0" topLeftCell="A1">
+      <selection pane="topLeft" activeCell="L25" sqref="L25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="4" max="4" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="40.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.8571428571429" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="40.7142857142857" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" ht="15">
       <c r="A1" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" ht="15">
       <c r="A2" t="s">
         <v>71</v>
       </c>
@@ -6296,7 +6374,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" ht="15">
       <c r="A3" t="s">
         <v>165</v>
       </c>
@@ -6322,7 +6400,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" ht="15">
       <c r="A4" t="s">
         <v>165</v>
       </c>
@@ -6348,7 +6426,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" ht="15">
       <c r="A5" t="s">
         <v>165</v>
       </c>
@@ -6374,7 +6452,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" ht="15">
       <c r="A6" t="s">
         <v>165</v>
       </c>
@@ -6400,7 +6478,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" ht="15">
       <c r="A7" t="s">
         <v>165</v>
       </c>
@@ -6426,7 +6504,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" ht="15">
       <c r="A8" t="s">
         <v>137</v>
       </c>
@@ -6452,7 +6530,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" ht="15">
       <c r="A9" t="s">
         <v>137</v>
       </c>
@@ -6478,7 +6556,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" ht="15">
       <c r="A10" t="s">
         <v>137</v>
       </c>
@@ -6504,7 +6582,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" ht="15">
       <c r="A11" t="s">
         <v>137</v>
       </c>
@@ -6530,7 +6608,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" ht="15">
       <c r="A12" t="s">
         <v>137</v>
       </c>
@@ -6556,7 +6634,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" ht="15">
       <c r="A13" t="s">
         <v>137</v>
       </c>
@@ -6582,7 +6660,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" ht="15">
       <c r="A14" t="s">
         <v>137</v>
       </c>
@@ -6608,7 +6686,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" ht="15">
       <c r="A15" t="s">
         <v>137</v>
       </c>
@@ -6634,7 +6712,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" ht="15">
       <c r="A16" t="s">
         <v>137</v>
       </c>
@@ -6648,19 +6726,19 @@
         <v>123</v>
       </c>
       <c r="F16" t="s">
-        <v>15</v>
+        <v>649</v>
       </c>
       <c r="G16" t="s">
-        <v>15</v>
+        <v>649</v>
       </c>
       <c r="H16" t="s">
-        <v>15</v>
+        <v>649</v>
       </c>
       <c r="I16" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+        <v>650</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" ht="15">
       <c r="A17" t="s">
         <v>137</v>
       </c>
@@ -6686,7 +6764,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" ht="15">
       <c r="A18" t="s">
         <v>137</v>
       </c>
@@ -6712,7 +6790,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" ht="15">
       <c r="A19" t="s">
         <v>137</v>
       </c>
@@ -6738,7 +6816,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" ht="15">
       <c r="A20" t="s">
         <v>137</v>
       </c>
@@ -6764,7 +6842,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" ht="15">
       <c r="A21" t="s">
         <v>137</v>
       </c>
@@ -6790,7 +6868,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" ht="15">
       <c r="A22" t="s">
         <v>137</v>
       </c>
@@ -6816,7 +6894,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" ht="15">
       <c r="A23" t="s">
         <v>137</v>
       </c>
@@ -6830,19 +6908,19 @@
         <v>129</v>
       </c>
       <c r="F23" t="s">
-        <v>15</v>
+        <v>649</v>
       </c>
       <c r="G23" t="s">
-        <v>16</v>
+        <v>650</v>
       </c>
       <c r="H23" t="s">
-        <v>15</v>
+        <v>649</v>
       </c>
       <c r="I23" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+        <v>650</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" ht="15">
       <c r="A24" t="s">
         <v>137</v>
       </c>
@@ -6868,7 +6946,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" ht="15">
       <c r="A25" t="s">
         <v>137</v>
       </c>
@@ -6894,7 +6972,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" ht="15">
       <c r="A26" t="s">
         <v>137</v>
       </c>
@@ -6920,7 +6998,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" ht="15">
       <c r="A27" t="s">
         <v>137</v>
       </c>
@@ -6946,7 +7024,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" ht="15">
       <c r="A28" t="s">
         <v>137</v>
       </c>
@@ -6972,7 +7050,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" ht="15">
       <c r="A29" t="s">
         <v>137</v>
       </c>
@@ -6998,7 +7076,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" ht="15">
       <c r="A30" t="s">
         <v>137</v>
       </c>
@@ -7024,7 +7102,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" ht="15">
       <c r="A31" t="s">
         <v>137</v>
       </c>
@@ -7050,7 +7128,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9" ht="15">
       <c r="A32" t="s">
         <v>137</v>
       </c>
@@ -7076,7 +7154,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:9" ht="15">
       <c r="A33" t="s">
         <v>137</v>
       </c>
@@ -7102,7 +7180,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:9" ht="15">
       <c r="A34" t="s">
         <v>137</v>
       </c>
@@ -7128,7 +7206,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:9" ht="15">
       <c r="A35" t="s">
         <v>137</v>
       </c>
@@ -7154,7 +7232,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:9" ht="15">
       <c r="A36" t="s">
         <v>137</v>
       </c>
@@ -7180,7 +7258,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:9" ht="15">
       <c r="A37" t="s">
         <v>137</v>
       </c>
@@ -7206,7 +7284,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:9" ht="15">
       <c r="A38" t="s">
         <v>137</v>
       </c>
@@ -7232,7 +7310,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:9" ht="15">
       <c r="A39" t="s">
         <v>137</v>
       </c>
@@ -7258,7 +7336,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:9" ht="15">
       <c r="A40" t="s">
         <v>137</v>
       </c>
@@ -7284,7 +7362,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:9" ht="15">
       <c r="A41" t="s">
         <v>137</v>
       </c>
@@ -7310,7 +7388,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:9" ht="15">
       <c r="A42" t="s">
         <v>137</v>
       </c>
@@ -7336,7 +7414,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:9" ht="15">
       <c r="A43" t="s">
         <v>137</v>
       </c>
@@ -7362,7 +7440,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:9" ht="15">
       <c r="A44" t="s">
         <v>137</v>
       </c>
@@ -7388,7 +7466,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:9" ht="15">
       <c r="A45" t="s">
         <v>137</v>
       </c>
@@ -7414,7 +7492,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:9" ht="15">
       <c r="A46" t="s">
         <v>137</v>
       </c>
@@ -7440,7 +7518,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:9" ht="15">
       <c r="A47" t="s">
         <v>137</v>
       </c>
@@ -7466,7 +7544,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:9" ht="15">
       <c r="A48" t="s">
         <v>137</v>
       </c>
@@ -7492,7 +7570,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:9" ht="15">
       <c r="A49" t="s">
         <v>137</v>
       </c>
@@ -7518,7 +7596,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:9" ht="15">
       <c r="A50" t="s">
         <v>137</v>
       </c>
@@ -7544,7 +7622,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:9" ht="15">
       <c r="A51" t="s">
         <v>137</v>
       </c>
@@ -7570,7 +7648,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:9" ht="15">
       <c r="A52" t="s">
         <v>137</v>
       </c>
@@ -7596,7 +7674,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:9" ht="15">
       <c r="A53" t="s">
         <v>137</v>
       </c>
@@ -7622,7 +7700,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:9" ht="15">
       <c r="A54" t="s">
         <v>137</v>
       </c>
@@ -7648,7 +7726,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:9" ht="15">
       <c r="A55" t="s">
         <v>137</v>
       </c>
@@ -7674,7 +7752,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:9" ht="15">
       <c r="A56" t="s">
         <v>137</v>
       </c>
@@ -7700,7 +7778,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:9" ht="15">
       <c r="A57" t="s">
         <v>137</v>
       </c>
@@ -7726,7 +7804,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:9" ht="15">
       <c r="A58" t="s">
         <v>137</v>
       </c>
@@ -7752,7 +7830,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:9" ht="15">
       <c r="A59" t="s">
         <v>137</v>
       </c>
@@ -7778,7 +7856,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:9" ht="15">
       <c r="A60" t="s">
         <v>137</v>
       </c>
@@ -7804,7 +7882,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:9" ht="15">
       <c r="A61" t="s">
         <v>137</v>
       </c>
@@ -7830,7 +7908,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:9" ht="15">
       <c r="A62" t="s">
         <v>137</v>
       </c>
@@ -7856,7 +7934,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:9" ht="15">
       <c r="A63" t="s">
         <v>137</v>
       </c>
@@ -7882,7 +7960,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:9" ht="15">
       <c r="A64" t="s">
         <v>137</v>
       </c>
@@ -7908,7 +7986,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:9" ht="15">
       <c r="A65" t="s">
         <v>163</v>
       </c>
@@ -7934,7 +8012,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:9" ht="15">
       <c r="A66" t="s">
         <v>163</v>
       </c>
@@ -7960,7 +8038,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:9" ht="15">
       <c r="A67" t="s">
         <v>163</v>
       </c>
@@ -7986,7 +8064,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:9" ht="15">
       <c r="A68" t="s">
         <v>163</v>
       </c>
@@ -8012,7 +8090,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:9" ht="15">
       <c r="A69" t="s">
         <v>163</v>
       </c>
@@ -8038,7 +8116,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:9" ht="15">
       <c r="A70" t="s">
         <v>163</v>
       </c>
@@ -8064,7 +8142,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:9" ht="15">
       <c r="A71" t="s">
         <v>163</v>
       </c>
@@ -8090,7 +8168,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:9" ht="15">
       <c r="A72" t="s">
         <v>163</v>
       </c>
@@ -8116,7 +8194,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:9" ht="15">
       <c r="A73" t="s">
         <v>163</v>
       </c>
@@ -8142,7 +8220,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:9" ht="15">
       <c r="A74" t="s">
         <v>163</v>
       </c>
@@ -8168,7 +8246,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:9" ht="15">
       <c r="A75" t="s">
         <v>163</v>
       </c>
@@ -8194,7 +8272,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:9" ht="15">
       <c r="A76" t="s">
         <v>163</v>
       </c>
@@ -8220,7 +8298,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:9" ht="15">
       <c r="A77" t="s">
         <v>163</v>
       </c>
@@ -8246,7 +8324,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="78" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:9" ht="15">
       <c r="A78" t="s">
         <v>163</v>
       </c>
@@ -8272,7 +8350,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="79" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:9" ht="15">
       <c r="A79" t="s">
         <v>163</v>
       </c>
@@ -8304,28 +8382,28 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DFD40ADC-D5CC-4772-80B1-A116F59E0A06}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DFD40ADC-D5CC-4772-80B1-A116F59E0A06}">
   <sheetPr codeName="Sheet2">
     <tabColor rgb="FF92D050"/>
   </sheetPr>
   <dimension ref="A1:L20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F28" sqref="F28"/>
+    <sheetView workbookViewId="0" topLeftCell="A1">
+      <selection pane="topLeft" activeCell="F28" sqref="F28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="6" max="6" width="19.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="40.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.4285714285714" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="40.4285714285714" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" ht="15">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" ht="15">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -8363,7 +8441,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" ht="15">
       <c r="A3" t="s">
         <v>191</v>
       </c>
@@ -8389,7 +8467,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" ht="15">
       <c r="A4" t="s">
         <v>191</v>
       </c>
@@ -8415,7 +8493,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" ht="15">
       <c r="A5" t="s">
         <v>191</v>
       </c>
@@ -8441,7 +8519,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" ht="15">
       <c r="A6" t="s">
         <v>191</v>
       </c>
@@ -8467,7 +8545,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:11" ht="15">
       <c r="B7" t="s">
         <v>348</v>
       </c>
@@ -8490,7 +8568,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:11" ht="15">
       <c r="B8" t="s">
         <v>543</v>
       </c>
@@ -8513,7 +8591,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:11" ht="15">
       <c r="B9" t="s">
         <v>244</v>
       </c>
@@ -8536,7 +8614,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:11" ht="15">
       <c r="B10" t="s">
         <v>58</v>
       </c>
@@ -8559,7 +8637,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:11" ht="15">
       <c r="B11" t="s">
         <v>59</v>
       </c>
@@ -8582,7 +8660,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:11" ht="15">
       <c r="B12" t="s">
         <v>60</v>
       </c>
@@ -8605,7 +8683,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:11" ht="15">
       <c r="B13" t="s">
         <v>61</v>
       </c>
@@ -8628,7 +8706,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:11" ht="15">
       <c r="B14" t="s">
         <v>631</v>
       </c>
@@ -8651,7 +8729,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:11" ht="15">
       <c r="B15" t="s">
         <v>629</v>
       </c>
@@ -8674,7 +8752,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" ht="15">
       <c r="A16" s="1" t="s">
         <v>325</v>
       </c>
@@ -8700,7 +8778,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:11" ht="15">
       <c r="B17" t="s">
         <v>627</v>
       </c>
@@ -8723,7 +8801,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:11" ht="15">
       <c r="B18" t="s">
         <v>626</v>
       </c>
@@ -8746,7 +8824,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:11" ht="15">
       <c r="B19" t="s">
         <v>632</v>
       </c>
@@ -8769,7 +8847,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" ht="15">
       <c r="A20" s="1" t="s">
         <v>325</v>
       </c>
@@ -8801,28 +8879,28 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24231217-6A54-4B12-AA31-B59CB94B1CCE}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24231217-6A54-4B12-AA31-B59CB94B1CCE}">
   <sheetPr codeName="Sheet3">
     <tabColor rgb="FF92D050"/>
   </sheetPr>
   <dimension ref="A1:L16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+    <sheetView workbookViewId="0" topLeftCell="A1">
+      <selection pane="topLeft" activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="6" max="6" width="19.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="40.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.4285714285714" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="40.4285714285714" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" ht="15">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" ht="15">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -8860,7 +8938,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" ht="15">
       <c r="A3" t="s">
         <v>45</v>
       </c>
@@ -8886,7 +8964,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" ht="15">
       <c r="A4" t="s">
         <v>45</v>
       </c>
@@ -8912,7 +8990,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" ht="15">
       <c r="A5" t="s">
         <v>45</v>
       </c>
@@ -8938,7 +9016,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" ht="15">
       <c r="A6" t="s">
         <v>45</v>
       </c>
@@ -8964,7 +9042,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" ht="15">
       <c r="A7" t="s">
         <v>45</v>
       </c>
@@ -8990,7 +9068,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" ht="15">
       <c r="A8" t="s">
         <v>45</v>
       </c>
@@ -9016,7 +9094,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" ht="15">
       <c r="A9" t="s">
         <v>45</v>
       </c>
@@ -9042,7 +9120,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" ht="15">
       <c r="A10" t="s">
         <v>45</v>
       </c>
@@ -9068,7 +9146,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" ht="15">
       <c r="A11" t="s">
         <v>45</v>
       </c>
@@ -9094,7 +9172,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" ht="15">
       <c r="A12" t="s">
         <v>45</v>
       </c>
@@ -9120,7 +9198,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" ht="15">
       <c r="A13" t="s">
         <v>45</v>
       </c>
@@ -9146,7 +9224,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" ht="15">
       <c r="A14" t="s">
         <v>45</v>
       </c>
@@ -9172,7 +9250,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" ht="15">
       <c r="A15" t="s">
         <v>45</v>
       </c>
@@ -9198,7 +9276,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" ht="15">
       <c r="A16" t="s">
         <v>45</v>
       </c>
@@ -9230,30 +9308,30 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73E260F6-B56C-4203-813B-A6591E1CBE42}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73E260F6-B56C-4203-813B-A6591E1CBE42}">
   <sheetPr codeName="Sheet4">
     <tabColor rgb="FF92D050"/>
   </sheetPr>
   <dimension ref="A1:L22"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0" topLeftCell="A1">
+      <selection pane="topLeft" activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="41.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="34.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="25.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="67.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="41.4285714285714" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="34.1428571428571" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="25.5714285714286" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="67.5714285714286" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" ht="15">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" ht="15">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -9291,7 +9369,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:11" ht="15">
       <c r="B3" t="s">
         <v>200</v>
       </c>
@@ -9314,7 +9392,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:11" ht="15">
       <c r="B4" t="s">
         <v>199</v>
       </c>
@@ -9337,7 +9415,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:11" ht="15">
       <c r="B5" t="s">
         <v>198</v>
       </c>
@@ -9360,7 +9438,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:11" ht="15">
       <c r="B6" t="s">
         <v>197</v>
       </c>
@@ -9383,7 +9461,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:11" ht="15">
       <c r="B7" t="s">
         <v>196</v>
       </c>
@@ -9406,7 +9484,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:11" ht="15">
       <c r="B8" t="s">
         <v>195</v>
       </c>
@@ -9429,7 +9507,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:11" ht="15">
       <c r="B9" t="s">
         <v>194</v>
       </c>
@@ -9452,7 +9530,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:11" ht="15">
       <c r="B10" t="s">
         <v>193</v>
       </c>
@@ -9475,7 +9553,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:11" ht="15">
       <c r="B11" t="s">
         <v>192</v>
       </c>
@@ -9498,7 +9576,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" ht="15">
       <c r="A12" s="1" t="s">
         <v>325</v>
       </c>
@@ -9527,7 +9605,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" ht="15">
       <c r="A13" s="1" t="str">
         <f>$F$12</f>
         <v>RSD_BLD-XXX_NRGSRV-WS</v>
@@ -9554,9 +9632,9 @@
         <v>16</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" ht="15">
       <c r="A14" s="1" t="str">
-        <f t="shared" ref="A14:A15" si="0">$F$12</f>
+        <f t="shared" si="0" ref="A14:A15">$F$12</f>
         <v>RSD_BLD-XXX_NRGSRV-WS</v>
       </c>
       <c r="B14" t="s">
@@ -9581,7 +9659,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" ht="15">
       <c r="A15" s="1" t="str">
         <f t="shared" si="0"/>
         <v>RSD_BLD-XXX_NRGSRV-WS</v>
@@ -9608,7 +9686,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" ht="15">
       <c r="A16" t="s">
         <v>45</v>
       </c>
@@ -9634,7 +9712,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" ht="15">
       <c r="A17" t="s">
         <v>45</v>
       </c>
@@ -9660,7 +9738,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" ht="15">
       <c r="A18" t="s">
         <v>45</v>
       </c>
@@ -9686,7 +9764,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" ht="15">
       <c r="A19" s="1"/>
       <c r="B19" t="s">
         <v>504</v>
@@ -9710,7 +9788,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" ht="15">
       <c r="A20" s="1" t="str">
         <f>$F$19</f>
         <v>RSD_BLD-XXX_RTFT</v>
@@ -9737,9 +9815,9 @@
         <v>16</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" ht="15">
       <c r="A21" s="1" t="str">
-        <f t="shared" ref="A21:A22" si="1">$F$19</f>
+        <f t="shared" si="1" ref="A21:A22">$F$19</f>
         <v>RSD_BLD-XXX_RTFT</v>
       </c>
       <c r="B21" t="s">
@@ -9764,7 +9842,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" ht="15">
       <c r="A22" s="1" t="str">
         <f t="shared" si="1"/>
         <v>RSD_BLD-XXX_RTFT</v>
@@ -9797,28 +9875,28 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{164F825B-1ED3-4C53-ABF7-18084792D4FD}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{164F825B-1ED3-4C53-ABF7-18084792D4FD}">
   <sheetPr codeName="Sheet5">
     <tabColor rgb="FF92D050"/>
   </sheetPr>
   <dimension ref="A1:L38"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:L3"/>
+    <sheetView workbookViewId="0" topLeftCell="A1">
+      <selection pane="topLeft" activeCell="A3" sqref="A3:L3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="6" max="6" width="24.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="58.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="24.1428571428571" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="58.1428571428571" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" ht="15">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" ht="15">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -9856,7 +9934,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" ht="15">
       <c r="A3" t="s">
         <v>45</v>
       </c>
@@ -9885,7 +9963,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" ht="15">
       <c r="A4" t="s">
         <v>45</v>
       </c>
@@ -9914,7 +9992,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" ht="15">
       <c r="A5" t="s">
         <v>45</v>
       </c>
@@ -9943,7 +10021,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" ht="15">
       <c r="A6" t="s">
         <v>45</v>
       </c>
@@ -9972,7 +10050,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" ht="15">
       <c r="A7" t="s">
         <v>45</v>
       </c>
@@ -10001,7 +10079,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" ht="15">
       <c r="A8" t="s">
         <v>45</v>
       </c>
@@ -10030,7 +10108,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" ht="15">
       <c r="A9" t="s">
         <v>45</v>
       </c>
@@ -10059,7 +10137,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" ht="15">
       <c r="A10" t="s">
         <v>45</v>
       </c>
@@ -10088,7 +10166,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" ht="15">
       <c r="A11" t="s">
         <v>45</v>
       </c>
@@ -10117,7 +10195,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" ht="15">
       <c r="A12" t="s">
         <v>45</v>
       </c>
@@ -10146,7 +10224,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" ht="15">
       <c r="A13" t="s">
         <v>45</v>
       </c>
@@ -10175,7 +10253,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" ht="15">
       <c r="A14" t="s">
         <v>45</v>
       </c>
@@ -10204,7 +10282,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" ht="15">
       <c r="A15" t="s">
         <v>45</v>
       </c>
@@ -10233,7 +10311,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" ht="15">
       <c r="A16" t="s">
         <v>45</v>
       </c>
@@ -10262,7 +10340,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" ht="15">
       <c r="A17" t="s">
         <v>45</v>
       </c>
@@ -10291,7 +10369,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" ht="15">
       <c r="A18" t="s">
         <v>45</v>
       </c>
@@ -10320,7 +10398,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" ht="15">
       <c r="A19" t="s">
         <v>45</v>
       </c>
@@ -10349,7 +10427,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" ht="15">
       <c r="A20" t="s">
         <v>45</v>
       </c>
@@ -10378,7 +10456,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" ht="15">
       <c r="A21" t="s">
         <v>45</v>
       </c>
@@ -10407,7 +10485,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" ht="15">
       <c r="A22" t="s">
         <v>45</v>
       </c>
@@ -10436,7 +10514,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" ht="15">
       <c r="A23" t="s">
         <v>45</v>
       </c>
@@ -10465,7 +10543,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" ht="15">
       <c r="A24" t="s">
         <v>45</v>
       </c>
@@ -10494,7 +10572,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" ht="15">
       <c r="A25" t="s">
         <v>45</v>
       </c>
@@ -10523,7 +10601,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" ht="15">
       <c r="A26" t="s">
         <v>45</v>
       </c>
@@ -10552,7 +10630,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" ht="15">
       <c r="A27" t="s">
         <v>45</v>
       </c>
@@ -10581,7 +10659,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11" ht="15">
       <c r="A28" t="s">
         <v>45</v>
       </c>
@@ -10610,7 +10688,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11" ht="15">
       <c r="A29" t="s">
         <v>45</v>
       </c>
@@ -10639,7 +10717,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11" ht="15">
       <c r="A30" t="s">
         <v>45</v>
       </c>
@@ -10668,7 +10746,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11" ht="15">
       <c r="A31" t="s">
         <v>45</v>
       </c>
@@ -10697,7 +10775,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11" ht="15">
       <c r="A32" t="s">
         <v>45</v>
       </c>
@@ -10726,7 +10804,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:11" ht="15">
       <c r="A33" t="s">
         <v>45</v>
       </c>
@@ -10755,7 +10833,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:11" ht="15">
       <c r="A34" t="s">
         <v>45</v>
       </c>
@@ -10784,7 +10862,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:11" ht="15">
       <c r="A35" t="s">
         <v>45</v>
       </c>
@@ -10813,7 +10891,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:11" ht="15">
       <c r="A36" t="s">
         <v>45</v>
       </c>
@@ -10842,7 +10920,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:11" ht="15">
       <c r="A37" t="s">
         <v>45</v>
       </c>
@@ -10871,7 +10949,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:11" ht="15">
       <c r="A38" t="s">
         <v>45</v>
       </c>
@@ -10906,28 +10984,28 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EEDDC4F5-4EDB-49DB-9D6D-333A351F1738}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EEDDC4F5-4EDB-49DB-9D6D-333A351F1738}">
   <sheetPr codeName="Sheet6">
     <tabColor rgb="FF92D050"/>
   </sheetPr>
   <dimension ref="A1:L19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="R9" sqref="R9"/>
+    <sheetView workbookViewId="0" topLeftCell="A1">
+      <selection pane="topLeft" activeCell="R9" sqref="R9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="6" max="6" width="19.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="53.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.4285714285714" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="53.2857142857143" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" ht="15">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" ht="15">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -10965,7 +11043,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:9" ht="15">
       <c r="B3" t="s">
         <v>360</v>
       </c>
@@ -10982,7 +11060,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:9" ht="15">
       <c r="B4" t="s">
         <v>361</v>
       </c>
@@ -10999,7 +11077,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:9" ht="15">
       <c r="B5" t="s">
         <v>350</v>
       </c>
@@ -11016,7 +11094,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:11" ht="15">
       <c r="B6" t="s">
         <v>362</v>
       </c>
@@ -11039,7 +11117,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:9" ht="15">
       <c r="B7" t="s">
         <v>363</v>
       </c>
@@ -11056,7 +11134,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:9" ht="15">
       <c r="B8" t="s">
         <v>365</v>
       </c>
@@ -11073,7 +11151,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:9" ht="15">
       <c r="B9" t="s">
         <v>364</v>
       </c>
@@ -11090,7 +11168,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:9" ht="15">
       <c r="B10" t="s">
         <v>62</v>
       </c>
@@ -11107,7 +11185,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:9" ht="15">
       <c r="B11" t="s">
         <v>63</v>
       </c>
@@ -11124,7 +11202,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:11" ht="15">
       <c r="B12" t="s">
         <v>64</v>
       </c>
@@ -11147,7 +11225,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:9" ht="15">
       <c r="B13" t="s">
         <v>349</v>
       </c>
@@ -11164,7 +11242,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:9" ht="15">
       <c r="B14" t="s">
         <v>65</v>
       </c>
@@ -11181,7 +11259,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:9" ht="15">
       <c r="B15" t="s">
         <v>66</v>
       </c>
@@ -11198,7 +11276,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:9" ht="15">
       <c r="B16" t="s">
         <v>67</v>
       </c>
@@ -11215,7 +11293,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="17" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:9" ht="15">
       <c r="B17" t="s">
         <v>68</v>
       </c>
@@ -11232,7 +11310,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:9" ht="15">
       <c r="B18" t="s">
         <v>69</v>
       </c>
@@ -11249,7 +11327,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="19" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:9" ht="15">
       <c r="B19" t="s">
         <v>369</v>
       </c>
@@ -11272,28 +11350,28 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{16A73284-DF56-4361-8316-EB8159A9346F}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{16A73284-DF56-4361-8316-EB8159A9346F}">
   <sheetPr codeName="Sheet7">
     <tabColor rgb="FF92D050"/>
   </sheetPr>
   <dimension ref="A1:L3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+    <sheetView workbookViewId="0" topLeftCell="A1">
+      <selection pane="topLeft" activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="6" max="6" width="19.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="53.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.4285714285714" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="53.2857142857143" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" ht="15">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" ht="15">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -11331,7 +11409,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" ht="15">
       <c r="A3" t="s">
         <v>190</v>
       </c>
@@ -11359,33 +11437,33 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" paperSize="9" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B790B4BC-8607-4508-A698-E46A5EB98EA7}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B790B4BC-8607-4508-A698-E46A5EB98EA7}">
   <sheetPr codeName="Sheet8">
     <tabColor rgb="FF92D050"/>
   </sheetPr>
   <dimension ref="A1:L3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H3" sqref="H3:K3"/>
+    <sheetView workbookViewId="0" topLeftCell="A1">
+      <selection pane="topLeft" activeCell="H3" sqref="H3:K3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="6" max="6" width="19.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="53.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.4285714285714" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="53.2857142857143" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" ht="15">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" ht="15">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -11423,7 +11501,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:11" ht="15">
       <c r="B3" t="s">
         <v>451</v>
       </c>

</xml_diff>